<commit_message>
initial work on circles
</commit_message>
<xml_diff>
--- a/source/GP-yearsofsupport.xlsx
+++ b/source/GP-yearsofsupport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32580" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="GP-Years of Support" sheetId="1" r:id="rId1"/>
@@ -21,27 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="198">
   <si>
-    <t>Start year</t>
-  </si>
-  <si>
-    <t>End year</t>
-  </si>
-  <si>
-    <t>Total Number of Years</t>
-  </si>
-  <si>
-    <t>Total Number of Grants</t>
-  </si>
-  <si>
-    <t>Grantee</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Discipline</t>
-  </si>
-  <si>
     <t>The Loft Literary Center</t>
   </si>
   <si>
@@ -613,6 +592,27 @@
   </si>
   <si>
     <t>http://www.studiomuseum.org/</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>grants</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1018,16 +1017,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="4" width="16.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="39.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" customWidth="1"/>
@@ -1035,25 +1035,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="45" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>191</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>192</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>193</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>197</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>196</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1071,13 +1071,13 @@
         <v>51</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1095,13 +1095,13 @@
         <v>48</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1119,13 +1119,13 @@
         <v>41</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1143,13 +1143,13 @@
         <v>41</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1167,13 +1167,13 @@
         <v>44</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1191,13 +1191,13 @@
         <v>78</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1215,13 +1215,13 @@
         <v>37</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1239,13 +1239,13 @@
         <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1263,13 +1263,13 @@
         <v>27</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1287,13 +1287,13 @@
         <v>33</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1311,13 +1311,13 @@
         <v>25</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1335,13 +1335,13 @@
         <v>25</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1359,13 +1359,13 @@
         <v>30</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1383,13 +1383,13 @@
         <v>27</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1407,13 +1407,13 @@
         <v>24</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1431,13 +1431,13 @@
         <v>25</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1455,13 +1455,13 @@
         <v>24</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1479,13 +1479,13 @@
         <v>25</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1503,13 +1503,13 @@
         <v>23</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G20" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1527,13 +1527,13 @@
         <v>22</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1551,13 +1551,13 @@
         <v>22</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1575,13 +1575,13 @@
         <v>22</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1599,13 +1599,13 @@
         <v>22</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1623,13 +1623,13 @@
         <v>22</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F25" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1647,13 +1647,13 @@
         <v>21</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1671,13 +1671,13 @@
         <v>21</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1695,13 +1695,13 @@
         <v>21</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G28" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1719,10 +1719,10 @@
         <v>21</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1740,13 +1740,13 @@
         <v>21</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1764,10 +1764,10 @@
         <v>20</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G31" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1785,13 +1785,13 @@
         <v>21</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G32" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1809,10 +1809,10 @@
         <v>20</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1830,13 +1830,13 @@
         <v>20</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F34" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G34" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1854,13 +1854,13 @@
         <v>20</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F35" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G35" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1878,13 +1878,13 @@
         <v>20</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G36" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1902,13 +1902,13 @@
         <v>19</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F37" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G37" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1926,13 +1926,13 @@
         <v>19</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F38" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1950,13 +1950,13 @@
         <v>19</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F39" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G39" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1974,13 +1974,13 @@
         <v>20</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F40" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G40" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1998,13 +1998,13 @@
         <v>19</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F41" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G41" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2022,13 +2022,13 @@
         <v>21</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G42" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2046,13 +2046,13 @@
         <v>18</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F43" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G43" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2070,13 +2070,13 @@
         <v>18</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F44" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G44" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2094,13 +2094,13 @@
         <v>17</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F45" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G45" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2118,10 +2118,10 @@
         <v>17</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G46" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2139,13 +2139,13 @@
         <v>19</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F47" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G47" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2163,13 +2163,13 @@
         <v>20</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F48" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G48" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2187,13 +2187,13 @@
         <v>17</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F49" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G49" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2211,13 +2211,13 @@
         <v>17</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F50" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G50" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2235,13 +2235,13 @@
         <v>17</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F51" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G51" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2259,13 +2259,13 @@
         <v>17</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F52" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G52" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2283,13 +2283,13 @@
         <v>16</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F53" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G53" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2307,13 +2307,13 @@
         <v>16</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F54" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G54" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2331,13 +2331,13 @@
         <v>20</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F55" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G55" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2355,13 +2355,13 @@
         <v>16</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F56" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G56" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2379,13 +2379,13 @@
         <v>17</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F57" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G57" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2403,13 +2403,13 @@
         <v>15</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F58" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G58" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2427,13 +2427,13 @@
         <v>23</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F59" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G59" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2451,13 +2451,13 @@
         <v>15</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F60" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G60" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2475,13 +2475,13 @@
         <v>15</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F61" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G61" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2499,10 +2499,10 @@
         <v>14</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G62" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2520,13 +2520,13 @@
         <v>14</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F63" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G63" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2544,13 +2544,13 @@
         <v>14</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F64" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G64" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2568,13 +2568,13 @@
         <v>17</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F65" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="G65" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2592,13 +2592,13 @@
         <v>14</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F66" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G66" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2616,13 +2616,13 @@
         <v>14</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F67" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G67" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2640,13 +2640,13 @@
         <v>13</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F68" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G68" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2664,13 +2664,13 @@
         <v>13</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F69" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G69" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2688,13 +2688,13 @@
         <v>13</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F70" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G70" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2712,13 +2712,13 @@
         <v>14</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F71" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="G71" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2736,13 +2736,13 @@
         <v>14</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F72" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G72" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2760,13 +2760,13 @@
         <v>18</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F73" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G73" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2784,13 +2784,13 @@
         <v>13</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F74" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G74" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2808,13 +2808,13 @@
         <v>19</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F75" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G75" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2832,13 +2832,13 @@
         <v>13</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F76" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G76" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2856,10 +2856,10 @@
         <v>12</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="G77" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2877,13 +2877,13 @@
         <v>12</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F78" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G78" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2901,10 +2901,10 @@
         <v>12</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="G79" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2922,10 +2922,10 @@
         <v>11</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G80" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2943,13 +2943,13 @@
         <v>11</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="F81" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="G81" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2967,10 +2967,10 @@
         <v>12</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G82" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2988,13 +2988,13 @@
         <v>11</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F83" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G83" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3012,13 +3012,13 @@
         <v>11</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F84" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G84" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -3036,13 +3036,13 @@
         <v>16</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F85" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G85" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -3060,13 +3060,13 @@
         <v>12</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F86" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G86" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -3084,10 +3084,10 @@
         <v>11</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G87" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -3105,13 +3105,13 @@
         <v>10</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F88" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G88" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -3129,13 +3129,13 @@
         <v>10</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F89" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G89" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -3153,13 +3153,13 @@
         <v>12</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F90" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G90" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -3177,13 +3177,13 @@
         <v>10</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F91" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G91" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -3201,13 +3201,13 @@
         <v>11</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F92" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G92" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -3225,13 +3225,13 @@
         <v>10</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G93" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -3249,13 +3249,13 @@
         <v>12</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="F94" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="G94" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -3273,10 +3273,10 @@
         <v>11</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="G95" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -3294,13 +3294,13 @@
         <v>10</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F96" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G96" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -3318,13 +3318,13 @@
         <v>10</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F97" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G97" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -3342,13 +3342,13 @@
         <v>10</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F98" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G98" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="99" spans="1:7">

</xml_diff>